<commit_message>
Before sharing project with Jose
</commit_message>
<xml_diff>
--- a/Sapflow_data_supporting/Sapflow_station_info.xlsx
+++ b/Sapflow_data_supporting/Sapflow_station_info.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/TMCF_analysis/Sapflow/Sapflow_data_supporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Sapflow/Sapflow_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E8237C0F-DA91-49CC-A1D0-22A1AD6A8BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C4BB9D-6E41-4E69-B774-4DC6B1A2FDD8}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E8237C0F-DA91-49CC-A1D0-22A1AD6A8BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BE4ED8-0278-4AF1-8FD7-8F93914A113D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MUX_ports2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1030,7 +1043,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1041,7 +1054,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating download options for app
</commit_message>
<xml_diff>
--- a/Sapflow_data_supporting/Sapflow_station_info.xlsx
+++ b/Sapflow_data_supporting/Sapflow_station_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Sapflow/Sapflow_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{E8237C0F-DA91-49CC-A1D0-22A1AD6A8BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36213E3E-3F99-47D6-A741-F7C0CBD97A54}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{E8237C0F-DA91-49CC-A1D0-22A1AD6A8BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A81E9BA2-6652-47B9-BDF6-94A908FDF626}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="60">
   <si>
     <t>Tree</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>51:56</t>
+  </si>
+  <si>
+    <t>49:54</t>
+  </si>
+  <si>
+    <t>55:60</t>
   </si>
 </sst>
 </file>
@@ -752,9 +758,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -792,7 +798,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -898,7 +904,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1040,7 +1046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1051,7 +1057,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1203,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>35</v>
@@ -1511,13 +1517,13 @@
         <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>

</xml_diff>